<commit_message>
Actualizacion FrameworkWeb con actualizacion de clases - Marisela
</commit_message>
<xml_diff>
--- a/web-automation-framework/src/main/resources/excel/MyFlight.xlsx
+++ b/web-automation-framework/src/main/resources/excel/MyFlight.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>TC1</t>
   </si>
@@ -47,7 +47,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +69,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -122,7 +132,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -139,7 +149,9 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>

</xml_diff>